<commit_message>
Atualização pdf parte 06
</commit_message>
<xml_diff>
--- a/ME613Cronograma2S2020.xlsx
+++ b/ME613Cronograma2S2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\AtividadesAcademicas\Ensino\Unicamp\202002\ME613\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ME613-UNICAMP.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="75">
   <si>
     <t>Cronograma de Aulas</t>
   </si>
@@ -222,6 +222,33 @@
   </si>
   <si>
     <t>Avaliação de curso</t>
+  </si>
+  <si>
+    <t>Sessões Sincronas</t>
+  </si>
+  <si>
+    <t># 1</t>
+  </si>
+  <si>
+    <t># 2</t>
+  </si>
+  <si>
+    <t># 3</t>
+  </si>
+  <si>
+    <t># 4</t>
+  </si>
+  <si>
+    <t>Videos</t>
+  </si>
+  <si>
+    <t>Benilton</t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rafael </t>
   </si>
 </sst>
 </file>
@@ -323,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -396,6 +423,13 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -403,6 +437,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -686,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,15 +736,16 @@
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
@@ -720,8 +758,14 @@
       <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>1</v>
       </c>
@@ -737,8 +781,14 @@
       <c r="E4" s="15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="37">
+        <v>44090</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <v>2</v>
       </c>
@@ -754,8 +804,17 @@
       <c r="E5" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="37">
+        <v>44095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>3</v>
       </c>
@@ -771,8 +830,14 @@
       <c r="E6" s="19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="37">
+        <v>44095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>4</v>
       </c>
@@ -788,8 +853,14 @@
       <c r="E7" s="19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>5</v>
       </c>
@@ -805,8 +876,11 @@
       <c r="E8" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>6</v>
       </c>
@@ -822,8 +896,14 @@
       <c r="E9" s="19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>7</v>
       </c>
@@ -839,8 +919,14 @@
       <c r="E10" s="19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
         <v>5</v>
       </c>
@@ -850,12 +936,13 @@
       <c r="C11" s="21">
         <v>44116</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="38"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="41"/>
+      <c r="F11" s="36"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>8</v>
       </c>
@@ -871,8 +958,11 @@
       <c r="E12" s="19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>9</v>
       </c>
@@ -882,12 +972,13 @@
       <c r="C13" s="23">
         <v>44123</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="37"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="40"/>
+      <c r="F13" s="42"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <v>10</v>
       </c>
@@ -903,9 +994,12 @@
       <c r="E14" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="33"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <v>11</v>
       </c>
@@ -921,8 +1015,11 @@
       <c r="E15" s="19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <v>12</v>
       </c>
@@ -938,8 +1035,11 @@
       <c r="E16" s="19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>5</v>
       </c>
@@ -949,12 +1049,13 @@
       <c r="C17" s="21">
         <v>44137</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="38"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="41"/>
+      <c r="F17" s="36"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <v>13</v>
       </c>
@@ -970,8 +1071,11 @@
       <c r="E18" s="19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>14</v>
       </c>
@@ -987,8 +1091,11 @@
       <c r="E19" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>15</v>
       </c>
@@ -1004,8 +1111,11 @@
       <c r="E20" s="19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <v>16</v>
       </c>
@@ -1021,8 +1131,11 @@
       <c r="E21" s="19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <v>17</v>
       </c>
@@ -1038,8 +1151,11 @@
       <c r="E22" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <v>18</v>
       </c>
@@ -1055,8 +1171,11 @@
       <c r="E23" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="20" t="s">
         <v>3</v>
@@ -1064,12 +1183,13 @@
       <c r="C24" s="21">
         <v>44160</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="38"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="41"/>
+      <c r="F24" s="36"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
         <v>19</v>
       </c>
@@ -1085,8 +1205,11 @@
       <c r="E25" s="19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
         <v>20</v>
       </c>
@@ -1102,8 +1225,11 @@
       <c r="E26" s="19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>5</v>
       </c>
@@ -1115,8 +1241,9 @@
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="19"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
         <v>21</v>
       </c>
@@ -1132,8 +1259,11 @@
       <c r="E28" s="19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
         <v>22</v>
       </c>
@@ -1149,8 +1279,11 @@
       <c r="E29" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
         <v>23</v>
       </c>
@@ -1166,8 +1299,11 @@
       <c r="E30" s="19" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
         <v>24</v>
       </c>
@@ -1183,8 +1319,11 @@
       <c r="E31" s="19" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="29">
         <v>25</v>
       </c>
@@ -1194,20 +1333,21 @@
       <c r="C32" s="23">
         <v>44188</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="37"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
+      <c r="E32" s="40"/>
+      <c r="F32" s="42"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="25">
         <v>26</v>
       </c>
@@ -1223,8 +1363,11 @@
       <c r="E34" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="30">
         <v>27</v>
       </c>
@@ -1240,11 +1383,14 @@
       <c r="E35" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="25">
         <v>28</v>
       </c>
@@ -1260,8 +1406,11 @@
       <c r="E36" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="25">
         <v>29</v>
       </c>
@@ -1277,8 +1426,11 @@
       <c r="E37" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>30</v>
       </c>
@@ -1288,12 +1440,13 @@
       <c r="C38" s="6">
         <v>44214</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="35"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="38"/>
+      <c r="F38" s="35"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>62</v>
       </c>
@@ -1303,10 +1456,11 @@
       <c r="C39" s="9">
         <v>44221</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="35"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>